<commit_message>
name added to file
</commit_message>
<xml_diff>
--- a/TestScript.xlsx
+++ b/TestScript.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BlueSky\GitHub\BlueSKYClone\BlueSkyGitTraining2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dami\Documents\GitHub\BlueSkyGitTraining2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39280F9-7252-48F8-A870-1E4F96F97EAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2820" windowWidth="14400" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="2820" windowWidth="14400" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -37,12 +36,18 @@
   </si>
   <si>
     <t>I don’t like your teaching!!! I love it!!!</t>
+  </si>
+  <si>
+    <t>Dami Sanyaolu</t>
+  </si>
+  <si>
+    <t>I love your teaching. Learnt a lot. Thanks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -353,16 +358,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -370,12 +379,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>